<commit_message>
Update des Schemas und der Teilnehmer
</commit_message>
<xml_diff>
--- a/CraZZZy Crash Challenge/CCC-Daten.xlsx
+++ b/CraZZZy Crash Challenge/CCC-Daten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\info\KaroStuff\CraZZZy Crash Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E380A-268B-42A7-8D65-BE0C8DF4A16E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93360C9-32BE-44F4-BBBA-25300CF12904}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="690" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teilnehmer" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="251">
   <si>
     <t>Teilnehmer</t>
   </si>
@@ -758,9 +758,6 @@
     <t>Cpxy</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Graf_Zahl</t>
   </si>
   <si>
@@ -780,6 +777,15 @@
   </si>
   <si>
     <t>Teilnahmen</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t>entfernt</t>
   </si>
 </sst>
 </file>
@@ -882,7 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -941,13 +947,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift 2" xfId="2" builtinId="17"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="19">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -968,21 +980,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1053,47 +1050,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G66" totalsRowCount="1">
-  <autoFilter ref="A1:G65" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:E51">
-    <sortCondition ref="A1:A51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G69" totalsRowCount="1">
+  <autoFilter ref="A1:G68" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:E54">
+    <sortCondition ref="A1:A54"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Teilnehmer" totalsRowLabel="Ergebnis"/>
-    <tableColumn id="7" xr3:uid="{92058238-585F-4C96-B2A3-0F26469434C9}" name="Teilnahmen" dataDxfId="6" totalsRowDxfId="5">
+    <tableColumn id="7" xr3:uid="{92058238-585F-4C96-B2A3-0F26469434C9}" name="Teilnahmen" totalsRowLabel="x" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CCC1" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CCC2" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CCC3" totalsRowFunction="count" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CCC4" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="CCC5" totalsRowFunction="count" dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CCC1" totalsRowFunction="custom" dataDxfId="4">
+      <totalsRowFormula>COUNTIF(Tabelle1[CCC1],$B69)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CCC2" totalsRowFunction="custom" dataDxfId="3">
+      <totalsRowFormula>COUNTIF(Tabelle1[CCC2],$B69)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CCC3" totalsRowFunction="custom" dataDxfId="2">
+      <totalsRowFormula>COUNTIF(Tabelle1[CCC3],$B69)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CCC4" totalsRowFunction="custom" dataDxfId="1">
+      <totalsRowFormula>COUNTIF(Tabelle1[CCC4],$B69)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="CCC5" totalsRowFunction="custom" dataDxfId="0">
+      <totalsRowFormula>COUNTIF(Tabelle1[CCC5],$B69)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:L152" totalsRowShown="0" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:L152" totalsRowShown="0" dataDxfId="18">
   <autoFilter ref="A1:L152" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A2:J70">
     <sortCondition ref="A37"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CCC"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Spieltag" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Spieler" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Strecke" dataDxfId="20" dataCellStyle="Link"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="ZZZ" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="CPs" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Richtung" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Rennen" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Züge p.S." dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Züge Ges." dataDxfId="14">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Spieltag" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Spieler" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Strecke" dataDxfId="15" dataCellStyle="Link"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="ZZZ" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="CPs" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Richtung" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Rennen" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Züge p.S." dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Züge Ges." dataDxfId="9">
       <calculatedColumnFormula>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Rating" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Kommentar" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Rating" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Kommentar" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1396,17 +1403,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1414,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1478,47 +1487,49 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1">
+        <v>244</v>
+      </c>
+      <c r="B4" s="22">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -1534,7 +1545,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -1550,58 +1561,54 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>232</v>
       </c>
       <c r="B10" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>45</v>
       </c>
@@ -1610,29 +1617,31 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>241</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B12" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1641,36 +1650,36 @@
         <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>237</v>
       </c>
       <c r="B13" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>45</v>
@@ -1680,7 +1689,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -1694,39 +1703,41 @@
         <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>3</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>45</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>234</v>
-      </c>
-      <c r="B17" s="1">
+        <v>246</v>
+      </c>
+      <c r="B17" s="22">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1734,41 +1745,39 @@
       <c r="F17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>230</v>
       </c>
       <c r="B18" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B19" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1778,7 +1787,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -1787,40 +1796,44 @@
       <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21" s="1">
+        <v>245</v>
+      </c>
+      <c r="B21" s="22">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="G21" s="1" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B22" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>45</v>
       </c>
@@ -1830,250 +1843,246 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
       <c r="B24" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>241</v>
       </c>
       <c r="B25" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
         <v>1</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="C27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>244</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>243</v>
-      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>4</v>
-      </c>
-      <c r="C31" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>236</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
         <v>2</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>243</v>
       </c>
       <c r="B33" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>236</v>
       </c>
       <c r="B35" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
         <v>2</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>5</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
         <v>45</v>
       </c>
@@ -2086,23 +2095,25 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B38" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -2120,115 +2131,121 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B39" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B40" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>243</v>
-      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B42" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>233</v>
+        <v>32</v>
       </c>
       <c r="B43" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B45" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -2246,29 +2263,27 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>233</v>
       </c>
       <c r="B46" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E46" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>45</v>
@@ -2276,41 +2291,31 @@
       <c r="D47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B48" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B49" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -2328,41 +2333,53 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B50" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B52" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
@@ -2380,13 +2397,15 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B53" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>0</v>
-      </c>
-      <c r="C53" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2394,141 +2413,143 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B54" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>3</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B55" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>243</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B56" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>5</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B58" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B59" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B60" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
         <v>1</v>
       </c>
-      <c r="C60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D60" s="1"/>
-      <c r="E60" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B61" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>45</v>
@@ -2536,65 +2557,49 @@
       <c r="D61" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B62" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>235</v>
+        <v>52</v>
       </c>
       <c r="B63" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E63" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B64" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>45</v>
@@ -2605,16 +2610,20 @@
       <c r="E64" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B65" s="1">
         <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>45</v>
@@ -2622,7 +2631,9 @@
       <c r="D65" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E65" s="1"/>
+      <c r="E65" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F65" s="1" t="s">
         <v>45</v>
       </c>
@@ -2632,57 +2643,129 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>235</v>
+      </c>
+      <c r="B66" s="1">
+        <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
+        <v>2</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="1">
+        <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
+        <v>3</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" s="1">
+        <f>COUNTIF(Tabelle1[[#This Row],[CCC1]:[CCC5]],"x")</f>
+        <v>3</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>239</v>
       </c>
-      <c r="C66" s="1">
-        <f>SUBTOTAL(103,Tabelle1[CCC1])</f>
+      <c r="B69" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69">
+        <f>COUNTIF(Tabelle1[CCC1],$B69)</f>
         <v>42</v>
       </c>
-      <c r="D66" s="1">
-        <f>SUBTOTAL(103,Tabelle1[CCC2])</f>
+      <c r="D69">
+        <f>COUNTIF(Tabelle1[CCC2],$B69)</f>
         <v>30</v>
       </c>
-      <c r="E66" s="1">
-        <f>SUBTOTAL(103,Tabelle1[CCC3])</f>
+      <c r="E69">
+        <f>COUNTIF(Tabelle1[CCC3],$B69)</f>
         <v>28</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F69">
+        <f>COUNTIF(Tabelle1[CCC4],$B69)</f>
+        <v>22</v>
+      </c>
+      <c r="G69">
+        <f>COUNTIF(Tabelle1[CCC5],$B69)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="F70">
+        <f>COUNTIF(Tabelle1[CCC4],$B70)</f>
+        <v>5</v>
+      </c>
+      <c r="G70">
+        <f>COUNTIF(Tabelle1[CCC5],$B70)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="F71">
+        <f>COUNTIF(Tabelle1[CCC4],$B71)</f>
+        <v>3</v>
+      </c>
+      <c r="G71">
+        <f>COUNTIF(Tabelle1[CCC5],$B71)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="F72">
         <f>SUBTOTAL(103,Tabelle1[CCC4])</f>
-        <v>25</v>
-      </c>
-      <c r="G66" s="1">
+        <v>30</v>
+      </c>
+      <c r="G72">
         <f>SUBTOTAL(103,Tabelle1[CCC5])</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CCC6 Fix: Removed "DerFlieger"
</commit_message>
<xml_diff>
--- a/CraZZZy Crash Challenge/CCC-Daten.xlsx
+++ b/CraZZZy Crash Challenge/CCC-Daten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\JVerkin\projects\KaroToolsCollection\CraZZZy Crash Challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\info\KaroToolsCollection\CraZZZy Crash Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B349B72-64C4-474A-B7A4-FC22153A41A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C771A19-9D9C-4C45-8486-A60584853D8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teilnehmer" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Rennanzahl" sheetId="4" r:id="rId4"/>
     <sheet name="Clustering" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="181029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,10 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -61,14 +58,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -2061,7 +2058,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2201,6 +2198,10 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -4835,7 +4836,7 @@
   <dimension ref="A1:S132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="J137" sqref="J137"/>
+      <selection activeCell="K120" sqref="K120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -10267,7 +10268,7 @@
 &amp; COUNTIF(INDIRECT("I"&amp;ROW()+1&amp;":I"&amp;(ROW()+Tabelle3[[#This Row],[Spieltag]]),TRUE),"8") &amp; " / "
 &amp; COUNTIF(INDIRECT("I"&amp;ROW()+1&amp;":I"&amp;(ROW()+Tabelle3[[#This Row],[Spieltag]]),TRUE),"9") &amp; " / "
 &amp; COUNTIF(INDIRECT("I"&amp;ROW()+1&amp;":I"&amp;(ROW()+Tabelle3[[#This Row],[Spieltag]]),TRUE),"10")</f>
-        <v>7 / 0 / 8 / 10 / 0 / 0 / 0 / 0</v>
+        <v>7 / 6 / 2 / 10 / 0 / 0 / 0 / 0</v>
       </c>
       <c r="E107" s="15"/>
       <c r="F107" s="14"/>
@@ -10284,7 +10285,7 @@
       <c r="J107" s="14"/>
       <c r="K107" s="14">
         <f>SUM(K108:K132)</f>
-        <v>840</v>
+        <v>868</v>
       </c>
       <c r="L107" s="16">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
@@ -11052,16 +11053,16 @@
       <c r="H122" s="49">
         <v>43</v>
       </c>
-      <c r="I122" s="49">
+      <c r="I122" s="33">
         <v>6</v>
       </c>
       <c r="J122" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>7</v>
       </c>
-      <c r="K122" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>25</v>
+      <c r="K122" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>24</v>
       </c>
       <c r="L122" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
@@ -11104,16 +11105,16 @@
       <c r="H123" s="49">
         <v>127</v>
       </c>
-      <c r="I123" s="49">
+      <c r="I123" s="33">
         <v>3</v>
       </c>
       <c r="J123" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>9</v>
       </c>
-      <c r="K123" s="48">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>50</v>
+      <c r="K123" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>48</v>
       </c>
       <c r="L123" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
@@ -11156,27 +11157,27 @@
       <c r="H124" s="49">
         <v>57</v>
       </c>
-      <c r="I124" s="49">
-        <v>5</v>
+      <c r="I124" s="53">
+        <v>4</v>
       </c>
       <c r="J124" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>5</v>
       </c>
-      <c r="K124" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>30</v>
+      <c r="K124" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>36</v>
       </c>
       <c r="L124" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
-        <v>342</v>
+        <v>273.59999999999997</v>
       </c>
       <c r="M124" s="50">
         <v>224</v>
       </c>
       <c r="N124" s="51">
         <f>Tabelle3[[#This Row],[Züge Ges.]]/N$107+Tabelle3[[#This Row],[Startverzögerung]]</f>
-        <v>309.5</v>
+        <v>292.39999999999998</v>
       </c>
       <c r="O124" s="26"/>
       <c r="P124" s="26"/>
@@ -11208,27 +11209,27 @@
       <c r="H125" s="49">
         <v>49</v>
       </c>
-      <c r="I125" s="49">
-        <v>5</v>
+      <c r="I125" s="53">
+        <v>4</v>
       </c>
       <c r="J125" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>5</v>
       </c>
-      <c r="K125" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>30</v>
+      <c r="K125" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>36</v>
       </c>
       <c r="L125" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
-        <v>294</v>
+        <v>235.2</v>
       </c>
       <c r="M125" s="50">
         <v>238</v>
       </c>
       <c r="N125" s="51">
         <f>Tabelle3[[#This Row],[Züge Ges.]]/N$107+Tabelle3[[#This Row],[Startverzögerung]]</f>
-        <v>311.5</v>
+        <v>296.8</v>
       </c>
       <c r="O125" s="26"/>
       <c r="P125" s="26"/>
@@ -11260,27 +11261,27 @@
       <c r="H126" s="55">
         <v>43</v>
       </c>
-      <c r="I126" s="55">
-        <v>5</v>
+      <c r="I126" s="60">
+        <v>4</v>
       </c>
       <c r="J126" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>6</v>
       </c>
-      <c r="K126" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>30</v>
+      <c r="K126" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>36</v>
       </c>
       <c r="L126" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
-        <v>258</v>
+        <v>206.4</v>
       </c>
       <c r="M126" s="50">
         <v>252</v>
       </c>
       <c r="N126" s="51">
         <f>Tabelle3[[#This Row],[Züge Ges.]]/N$107+Tabelle3[[#This Row],[Startverzögerung]]</f>
-        <v>316.5</v>
+        <v>303.60000000000002</v>
       </c>
       <c r="O126" s="26"/>
       <c r="P126" s="26"/>
@@ -11312,16 +11313,16 @@
       <c r="H127" s="49">
         <v>33</v>
       </c>
-      <c r="I127" s="49">
+      <c r="I127" s="33">
         <v>6</v>
       </c>
       <c r="J127" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>7</v>
       </c>
-      <c r="K127" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>25</v>
+      <c r="K127" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>24</v>
       </c>
       <c r="L127" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
@@ -11364,27 +11365,27 @@
       <c r="H128" s="49">
         <v>44</v>
       </c>
-      <c r="I128" s="49">
-        <v>5</v>
+      <c r="I128" s="53">
+        <v>4</v>
       </c>
       <c r="J128" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>6</v>
       </c>
-      <c r="K128" s="48">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>30</v>
+      <c r="K128" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>36</v>
       </c>
       <c r="L128" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
-        <v>264</v>
+        <v>211.2</v>
       </c>
       <c r="M128" s="50">
         <v>280</v>
       </c>
       <c r="N128" s="51">
         <f>Tabelle3[[#This Row],[Züge Ges.]]/N$107+Tabelle3[[#This Row],[Startverzögerung]]</f>
-        <v>346</v>
+        <v>332.8</v>
       </c>
       <c r="O128" s="26"/>
       <c r="P128" s="26"/>
@@ -11416,27 +11417,27 @@
       <c r="H129" s="49">
         <v>39</v>
       </c>
-      <c r="I129" s="49">
-        <v>5</v>
+      <c r="I129" s="53">
+        <v>4</v>
       </c>
       <c r="J129" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>5</v>
       </c>
-      <c r="K129" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>30</v>
+      <c r="K129" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>36</v>
       </c>
       <c r="L129" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
-        <v>234</v>
+        <v>187.2</v>
       </c>
       <c r="M129" s="50">
         <v>294</v>
       </c>
       <c r="N129" s="51">
         <f>Tabelle3[[#This Row],[Züge Ges.]]/N$107+Tabelle3[[#This Row],[Startverzögerung]]</f>
-        <v>352.5</v>
+        <v>340.8</v>
       </c>
       <c r="O129" s="26"/>
       <c r="P129" s="26"/>
@@ -11468,16 +11469,16 @@
       <c r="H130" s="49">
         <v>39</v>
       </c>
-      <c r="I130" s="49">
+      <c r="I130" s="33">
         <v>3</v>
       </c>
       <c r="J130" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>4</v>
       </c>
-      <c r="K130" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>50</v>
+      <c r="K130" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>48</v>
       </c>
       <c r="L130" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
@@ -11520,16 +11521,16 @@
       <c r="H131" s="49">
         <v>32</v>
       </c>
-      <c r="I131" s="49">
+      <c r="I131" s="33">
         <v>3</v>
       </c>
       <c r="J131" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>4</v>
       </c>
-      <c r="K131" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>50</v>
+      <c r="K131" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>48</v>
       </c>
       <c r="L131" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
@@ -11572,27 +11573,27 @@
       <c r="H132" s="49">
         <v>19</v>
       </c>
-      <c r="I132" s="49">
-        <v>5</v>
+      <c r="I132" s="53">
+        <v>4</v>
       </c>
       <c r="J132" s="49">
         <f>_xlfn.NUMBERVALUE(VLOOKUP( Tabelle3[[#This Row],[Map ID]],'Alle Karten'!H:J,3))</f>
         <v>5</v>
       </c>
-      <c r="K132" s="3">
-        <f>$I$107*6/Tabelle3[[#This Row],[Spieler]]</f>
-        <v>30</v>
+      <c r="K132" s="59">
+        <f>($I$107-1)*6/Tabelle3[[#This Row],[Spieler]]</f>
+        <v>36</v>
       </c>
       <c r="L132" s="7">
         <f>Tabelle3[[#This Row],[Spieler]]*Tabelle3[[#This Row],[Züge p.S.]]*1.2</f>
-        <v>114</v>
+        <v>91.2</v>
       </c>
       <c r="M132" s="50">
         <v>336</v>
       </c>
       <c r="N132" s="51">
         <f>Tabelle3[[#This Row],[Züge Ges.]]/N$107+Tabelle3[[#This Row],[Startverzögerung]]</f>
-        <v>364.5</v>
+        <v>358.8</v>
       </c>
       <c r="O132" s="26"/>
       <c r="P132" s="26"/>
@@ -24127,7 +24128,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>